<commit_message>
Added new user to sign up excel
</commit_message>
<xml_diff>
--- a/tec2med_tickeline_template.xlsx
+++ b/tec2med_tickeline_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pauloteixeira/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33FCE5A-0762-1840-A46D-2A49F614799F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A90001-F27E-4642-9687-FB8625DCC7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{4767ED66-79FD-D545-A7DC-C4C330E2614A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4767ED66-79FD-D545-A7DC-C4C330E2614A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>email</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>a@gmail.com</t>
+  </si>
+  <si>
+    <t>Afonso Hermenegildo</t>
+  </si>
+  <si>
+    <t>afonsosousah@tec2med.com</t>
   </si>
 </sst>
 </file>
@@ -130,10 +136,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -469,16 +476,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C3F078-0943-7A47-B20B-EF5479A5E543}">
-  <dimension ref="A2:C8"/>
+  <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
@@ -492,7 +499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18">
+    <row r="3" spans="1:3" ht="17.399999999999999">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -503,7 +510,7 @@
         <v>961234567</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18">
+    <row r="4" spans="1:3" ht="17.399999999999999">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -514,7 +521,7 @@
         <v>967890987</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18">
+    <row r="5" spans="1:3" ht="17.399999999999999">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -525,7 +532,7 @@
         <v>934567898</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18">
+    <row r="6" spans="1:3" ht="17.399999999999999">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -536,7 +543,7 @@
         <v>987651423</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18">
+    <row r="7" spans="1:3" ht="17.399999999999999">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -547,7 +554,7 @@
         <v>987162345</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18">
+    <row r="8" spans="1:3" ht="17.399999999999999">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -556,11 +563,23 @@
       </c>
       <c r="C8">
         <v>965234567</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17.399999999999999">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>912345678</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{260C4FBA-ADB4-BC4F-9E24-2537B47DAD80}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{896886C8-3D8E-4AAA-826F-561A7D905248}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>